<commit_message>
itt rohadjak meg az utolso
</commit_message>
<xml_diff>
--- a/WebprogramozásBeadandóHtmlCssBootstrap.xlsx
+++ b/WebprogramozásBeadandóHtmlCssBootstrap.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oravecz.botond\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\9.osztaly\programozás\webrogramozas\ricsi\Kabitoszeresoldal-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D93D280E-C8B2-4101-AA7D-00F5D54ECE36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6451CF78-0D26-41A3-BC78-A2C94E68ADA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Fedőlap" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="82">
   <si>
     <t>Neved:</t>
   </si>
@@ -302,6 +302,15 @@
   </si>
   <si>
     <t>Minden értékre (szín, méret) használj változókat.</t>
+  </si>
+  <si>
+    <t>Oravecz Botond, Rendek Richárd Zalán,</t>
+  </si>
+  <si>
+    <t>oravecz.botond@ckik.hu , rendek.richard.zalan@ckik.hu</t>
+  </si>
+  <si>
+    <t>Kábítószerek</t>
   </si>
 </sst>
 </file>
@@ -1197,6 +1206,18 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1240,18 +1261,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Ezres" xfId="1" builtinId="3"/>
@@ -8585,8 +8594,8 @@
   <sheetPr codeName="Munka1"/>
   <dimension ref="A1:J464"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8605,15 +8614,15 @@
   <sheetData>
     <row r="1" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="31"/>
-      <c r="B1" s="96" t="s">
+      <c r="B1" s="81" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
       <c r="I1" s="31"/>
       <c r="J1" s="31"/>
     </row>
@@ -8622,12 +8631,14 @@
       <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
+      <c r="C2" s="86" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
       <c r="I2" s="31"/>
       <c r="J2" s="31"/>
     </row>
@@ -8636,12 +8647,14 @@
       <c r="B3" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="84"/>
-      <c r="D3" s="83"/>
-      <c r="E3" s="83"/>
-      <c r="F3" s="83"/>
-      <c r="G3" s="83"/>
-      <c r="H3" s="83"/>
+      <c r="C3" s="88" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
       <c r="I3" s="31"/>
       <c r="J3" s="31"/>
     </row>
@@ -8650,12 +8663,14 @@
       <c r="B4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="82"/>
-      <c r="D4" s="88"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="88"/>
-      <c r="G4" s="88"/>
-      <c r="H4" s="89"/>
+      <c r="C4" s="86" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="92"/>
+      <c r="E4" s="92"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="93"/>
       <c r="I4" s="31"/>
       <c r="J4" s="31"/>
     </row>
@@ -8673,30 +8688,30 @@
     </row>
     <row r="6" spans="1:10" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31"/>
-      <c r="B6" s="87" t="s">
+      <c r="B6" s="91" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="87"/>
-      <c r="H6" s="87"/>
+      <c r="C6" s="91"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="91"/>
+      <c r="F6" s="91"/>
+      <c r="G6" s="91"/>
+      <c r="H6" s="91"/>
       <c r="I6" s="31"/>
       <c r="J6" s="31"/>
     </row>
     <row r="7" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="31"/>
-      <c r="B7" s="90" t="str">
+      <c r="B7" s="94" t="str">
         <f>CONCATENATE("Az irányelvek között vannak kiemelt (sárga háttérszínnel és félkövér kiemeléssel jelölt) elvek , amelyek betartására kiemelten figyelni kell! Az elégséges szinthez legalább ",D11," pontot el kell érni. A tanulói és tanári értékelés tekintetében, maximum 10 darab irányelvben lehet eltérés.")</f>
         <v>Az irányelvek között vannak kiemelt (sárga háttérszínnel és félkövér kiemeléssel jelölt) elvek , amelyek betartására kiemelten figyelni kell! Az elégséges szinthez legalább 20 pontot el kell érni. A tanulói és tanári értékelés tekintetében, maximum 10 darab irányelvben lehet eltérés.</v>
       </c>
-      <c r="C7" s="90"/>
-      <c r="D7" s="90"/>
-      <c r="E7" s="90"/>
-      <c r="F7" s="90"/>
-      <c r="G7" s="90"/>
-      <c r="H7" s="90"/>
+      <c r="C7" s="94"/>
+      <c r="D7" s="94"/>
+      <c r="E7" s="94"/>
+      <c r="F7" s="94"/>
+      <c r="G7" s="94"/>
+      <c r="H7" s="94"/>
       <c r="I7" s="31"/>
       <c r="J7" s="31"/>
     </row>
@@ -8728,68 +8743,68 @@
     </row>
     <row r="10" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="31"/>
-      <c r="B10" s="85" t="s">
+      <c r="B10" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="86"/>
+      <c r="C10" s="90"/>
       <c r="D10" s="78">
         <f>SUM(Irányelvek!G:G)</f>
         <v>80</v>
       </c>
       <c r="E10" s="31"/>
-      <c r="F10" s="94" t="s">
+      <c r="F10" s="98" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="94"/>
-      <c r="H10" s="94"/>
+      <c r="G10" s="98"/>
+      <c r="H10" s="98"/>
       <c r="I10" s="31"/>
       <c r="J10" s="31"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="31"/>
-      <c r="B11" s="98" t="s">
+      <c r="B11" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="C11" s="99"/>
+      <c r="C11" s="84"/>
       <c r="D11" s="79">
         <v>20</v>
       </c>
       <c r="E11" s="31"/>
-      <c r="F11" s="95"/>
-      <c r="G11" s="95"/>
-      <c r="H11" s="95"/>
+      <c r="F11" s="99"/>
+      <c r="G11" s="99"/>
+      <c r="H11" s="99"/>
       <c r="I11" s="31"/>
       <c r="J11" s="31"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="31"/>
-      <c r="B12" s="85" t="s">
+      <c r="B12" s="89" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="86"/>
+      <c r="C12" s="90"/>
       <c r="D12" s="78">
         <v>20</v>
       </c>
       <c r="E12" s="31"/>
-      <c r="F12" s="95"/>
-      <c r="G12" s="95"/>
-      <c r="H12" s="95"/>
+      <c r="F12" s="99"/>
+      <c r="G12" s="99"/>
+      <c r="H12" s="99"/>
       <c r="I12" s="31"/>
       <c r="J12" s="31"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="31"/>
-      <c r="B13" s="85" t="s">
+      <c r="B13" s="89" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="86"/>
+      <c r="C13" s="90"/>
       <c r="D13" s="78">
         <v>40</v>
       </c>
       <c r="E13" s="31"/>
-      <c r="F13" s="95"/>
-      <c r="G13" s="95"/>
-      <c r="H13" s="95"/>
+      <c r="F13" s="99"/>
+      <c r="G13" s="99"/>
+      <c r="H13" s="99"/>
       <c r="I13" s="31"/>
       <c r="J13" s="31"/>
     </row>
@@ -8799,9 +8814,9 @@
       <c r="C14" s="31"/>
       <c r="D14" s="31"/>
       <c r="E14" s="31"/>
-      <c r="F14" s="95"/>
-      <c r="G14" s="95"/>
-      <c r="H14" s="95"/>
+      <c r="F14" s="99"/>
+      <c r="G14" s="99"/>
+      <c r="H14" s="99"/>
       <c r="I14" s="31"/>
       <c r="J14" s="31"/>
     </row>
@@ -8821,10 +8836,10 @@
     </row>
     <row r="16" spans="1:10" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="31"/>
-      <c r="B16" s="85" t="s">
+      <c r="B16" s="89" t="s">
         <v>39</v>
       </c>
-      <c r="C16" s="86"/>
+      <c r="C16" s="90"/>
       <c r="D16" s="30" t="b">
         <f t="array" ref="D16">IF(COUNTIFS(Irányelvek!D2:D39,"=hamis",Irányelvek!F2:F39,"=Igaz")=0,TRUE,FALSE)</f>
         <v>1</v>
@@ -8838,74 +8853,74 @@
     </row>
     <row r="17" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="31"/>
-      <c r="B17" s="85" t="s">
+      <c r="B17" s="89" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="86"/>
+      <c r="C17" s="90"/>
       <c r="D17" s="33">
         <f>SUM(Irányelvek!H2:H39)</f>
         <v>80</v>
       </c>
       <c r="E17" s="31"/>
-      <c r="F17" s="93" t="str">
+      <c r="F17" s="97" t="str">
         <f>VLOOKUP(D20,Ponthatárok!$C$3:$D$7,2,TRUE)</f>
         <v>Jeles (5)</v>
       </c>
-      <c r="G17" s="93"/>
-      <c r="H17" s="93"/>
+      <c r="G17" s="97"/>
+      <c r="H17" s="97"/>
       <c r="I17" s="31"/>
       <c r="J17" s="31"/>
     </row>
     <row r="18" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31"/>
-      <c r="B18" s="91" t="s">
+      <c r="B18" s="95" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="92"/>
+      <c r="C18" s="96"/>
       <c r="D18" s="36">
         <f>IF(D17&gt;D11,VLOOKUP(SUM(Irányelvek!J2:J39),Ponthatárok!G2:H12,2,TRUE),0)</f>
         <v>20</v>
       </c>
       <c r="E18" s="31"/>
-      <c r="F18" s="93"/>
-      <c r="G18" s="93"/>
-      <c r="H18" s="93"/>
+      <c r="F18" s="97"/>
+      <c r="G18" s="97"/>
+      <c r="H18" s="97"/>
       <c r="I18" s="31"/>
       <c r="J18" s="31"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="31"/>
-      <c r="B19" s="85" t="s">
+      <c r="B19" s="89" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="86"/>
+      <c r="C19" s="90"/>
       <c r="D19" s="80">
         <v>40</v>
       </c>
       <c r="E19" s="31"/>
-      <c r="F19" s="93"/>
-      <c r="G19" s="93"/>
-      <c r="H19" s="93"/>
+      <c r="F19" s="97"/>
+      <c r="G19" s="97"/>
+      <c r="H19" s="97"/>
       <c r="I19" s="31"/>
       <c r="J19" s="31"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="31"/>
-      <c r="B20" s="85" t="s">
+      <c r="B20" s="89" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="86"/>
+      <c r="C20" s="90"/>
       <c r="D20" s="33">
         <f>SUM(D17:D19)</f>
         <v>140</v>
       </c>
       <c r="E20" s="31"/>
-      <c r="F20" s="81" t="str">
+      <c r="F20" s="85" t="str">
         <f>CONCATENATE("Az önértékelés alapján ",VLOOKUP(D20,Ponthatárok!$C$3:$D$7,2,TRUE), "  érdemjegyet kapnál rá.")</f>
         <v>Az önértékelés alapján Jeles (5)  érdemjegyet kapnál rá.</v>
       </c>
-      <c r="G20" s="81"/>
-      <c r="H20" s="81"/>
+      <c r="G20" s="85"/>
+      <c r="H20" s="85"/>
       <c r="I20" s="31"/>
       <c r="J20" s="31"/>
     </row>
@@ -9356,6 +9371,8 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="Pt2r10NfCQvSDRx8qMjGYxYpEYBoOyIK56jWLg5u88pMtB0yZv+L45h/PZkvP5rgD0XQukcG0FY9SUv/PUWVng==" saltValue="OS0FMTO/1nXUT8EsxtE52w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="18">
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B16:C16"/>
     <mergeCell ref="B1:H1"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="F20:H20"/>
@@ -9372,8 +9389,6 @@
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="F17:H19"/>
     <mergeCell ref="F10:H14"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B16:C16"/>
   </mergeCells>
   <conditionalFormatting sqref="D17:D20">
     <cfRule type="expression" dxfId="2" priority="1" stopIfTrue="1">
@@ -9394,9 +9409,9 @@
   <sheetPr codeName="Munka2"/>
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>